<commit_message>
﻿Clean up system and update columns in patient xlsx
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/PatientValidationData.xlsx
+++ b/data/human/adult/validation/PatientValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\documentation\source\data\human\adult\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22088840-7D2F-4C99-A4CA-F510B1764C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F19EEEC-DEB1-4AB2-86C3-4F83734F2CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21630" yWindow="7365" windowWidth="30555" windowHeight="21255" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="28800" windowHeight="16920" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient-Validation" sheetId="33" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="66">
   <si>
     <t>Output</t>
   </si>
@@ -130,9 +130,6 @@
     <t>TotalMetabolicRate</t>
   </si>
   <si>
-    <t>ResultsFile</t>
-  </si>
-  <si>
     <t>MeanArterialPressure</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
     <t>Patient2SystemMean</t>
   </si>
   <si>
-    <t>MantissaDigits</t>
-  </si>
-  <si>
     <t>1f</t>
   </si>
   <si>
@@ -215,13 +209,22 @@
   </si>
   <si>
     <t>Compare the (expected) value computed by SetupPatient to the patient variable, which is updated every timestep in the engine</t>
+  </si>
+  <si>
+    <t>Table Precision</t>
+  </si>
+  <si>
+    <t>Request Type</t>
+  </si>
+  <si>
+    <t>Request Precision</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,8 +385,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -585,6 +596,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor rgb="FF000080"/>
       </patternFill>
     </fill>
   </fills>
@@ -776,7 +793,7 @@
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -821,6 +838,10 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1166,9 +1187,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="R25" sqref="R25"/>
     </sheetView>
@@ -1187,12 +1208,11 @@
     <col min="10" max="10" width="5.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.7109375" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1203,10 +1223,10 @@
         <v>31</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>2</v>
@@ -1218,7 +1238,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>6</v>
@@ -1232,14 +1252,17 @@
       <c r="M1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1255,12 +1278,13 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="15"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N2" s="15"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1274,10 +1298,11 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="15"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N3" s="15"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
@@ -1293,10 +1318,11 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="15"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N4" s="15"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
@@ -1312,10 +1338,11 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="15"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N5" s="15"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
@@ -1331,12 +1358,13 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="15"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N6" s="15"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -1350,12 +1378,13 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="15"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N7" s="15"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1369,10 +1398,11 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="15"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N8" s="15"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>32</v>
       </c>
@@ -1388,12 +1418,13 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="15"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N9" s="15"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1407,12 +1438,13 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="15"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N10" s="15"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -1426,12 +1458,13 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="15"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N11" s="15"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1445,12 +1478,13 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="15"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N12" s="15"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="12"/>
@@ -1464,14 +1498,15 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N13" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="12"/>
@@ -1485,10 +1520,11 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="15"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N14" s="15"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>29</v>
       </c>
@@ -1504,10 +1540,11 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="15"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N15" s="15"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>30</v>
       </c>
@@ -1523,10 +1560,11 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="15"/>
-    </row>
-    <row r="17" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="N16" s="15"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+    </row>
+    <row r="17" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>25</v>
       </c>
@@ -1534,7 +1572,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
@@ -1546,53 +1584,55 @@
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="N17" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+    </row>
+    <row r="18" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="N18" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+    </row>
+    <row r="19" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>26</v>
       </c>
@@ -1600,32 +1640,33 @@
         <v>4</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="N19" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+    </row>
+    <row r="20" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>15</v>
       </c>
@@ -1633,32 +1674,33 @@
         <v>10</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="N20" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+    </row>
+    <row r="21" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>18</v>
       </c>
@@ -1666,34 +1708,35 @@
         <v>4</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N21" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -1707,10 +1750,11 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="15"/>
-    </row>
-    <row r="23" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="N22" s="15"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+    </row>
+    <row r="23" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>33</v>
       </c>
@@ -1718,32 +1762,33 @@
         <v>10</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="N23" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+    </row>
+    <row r="24" spans="1:16" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>20</v>
       </c>
@@ -1751,73 +1796,75 @@
         <v>4</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="N24" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+    </row>
+    <row r="25" spans="1:16" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>34</v>
       </c>
       <c r="H25" s="11"/>
       <c r="I25" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="N25" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O25" s="17"/>
+      <c r="P25" s="17"/>
+    </row>
+    <row r="26" spans="1:16" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
@@ -1829,28 +1876,29 @@
       </c>
       <c r="H26" s="14"/>
       <c r="I26" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="N26" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+    </row>
+    <row r="27" spans="1:16" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
@@ -1862,28 +1910,29 @@
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J27" s="3"/>
       <c r="K27" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="N27" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+    </row>
+    <row r="28" spans="1:16" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
@@ -1895,28 +1944,29 @@
       </c>
       <c r="H28" s="14"/>
       <c r="I28" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="N28" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+    </row>
+    <row r="29" spans="1:16" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
@@ -1928,28 +1978,29 @@
       </c>
       <c r="H29" s="14"/>
       <c r="I29" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="N29" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+    </row>
+    <row r="30" spans="1:16" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
@@ -1961,28 +2012,29 @@
       </c>
       <c r="H30" s="14"/>
       <c r="I30" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N30" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+    </row>
+    <row r="31" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
@@ -1994,28 +2046,29 @@
       </c>
       <c r="H31" s="14"/>
       <c r="I31" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="48.75" x14ac:dyDescent="0.25">
+      <c r="N31" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+    </row>
+    <row r="32" spans="1:16" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
@@ -2027,18 +2080,19 @@
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="15" t="s">
-        <v>54</v>
-      </c>
+      <c r="N32" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>